<commit_message>
update test cases 12.29
</commit_message>
<xml_diff>
--- a/data/pool.xlsx
+++ b/data/pool.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="192">
   <si>
     <t>send command</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -715,6 +715,18 @@
   </si>
   <si>
     <t>checkpoint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">different types of pd can not compose the one pool </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pool -a expand -i 0 -p 6,16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fail to create Pool</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2063,10 +2075,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2087,19 +2099,19 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
+      <c r="A2" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
@@ -2110,7 +2122,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -2121,7 +2133,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>40</v>
@@ -2132,7 +2144,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -2143,7 +2155,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -2154,51 +2166,51 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>41</v>
@@ -2209,18 +2221,18 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
@@ -2231,7 +2243,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -2242,7 +2254,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
@@ -2253,7 +2265,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -2264,7 +2276,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
@@ -2275,7 +2287,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
@@ -2286,7 +2298,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
@@ -2297,7 +2309,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -2308,7 +2320,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
@@ -2319,7 +2331,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
@@ -2330,7 +2342,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -2341,7 +2353,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
@@ -2352,12 +2364,23 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>182</v>
       </c>
-      <c r="B26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>